<commit_message>
Update An example of Test Documentation.xlsx
Changing the title in the bug report.
</commit_message>
<xml_diff>
--- a/test_documentation/An example of Test Documentation.xlsx
+++ b/test_documentation/An example of Test Documentation.xlsx
@@ -217,9 +217,6 @@
     </r>
   </si>
   <si>
-    <t>BUG-00001: Ввод некорректной даты, в поле "Дата рождения", не приводит к ошибке.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -363,6 +360,9 @@
       </rPr>
       <t>An example of Test Documentation_BUG-00001.PNG</t>
     </r>
+  </si>
+  <si>
+    <t>BUG-00001: Ввод значения, в поле "Дата рождения", не приводит к ошибке.</t>
   </si>
 </sst>
 </file>
@@ -966,6 +966,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -974,18 +982,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1003,6 +999,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1217,7 +1217,7 @@
   <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:H7"/>
+      <selection activeCell="G3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1233,11 +1233,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,10 +1267,10 @@
       <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:11" ht="114" thickBot="1">
       <c r="A3" s="7">
@@ -1291,10 +1291,10 @@
       <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="55"/>
+      <c r="H3" s="53"/>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" ht="48.6">
@@ -1316,8 +1316,8 @@
       <c r="F4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
       <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:11" ht="81">
@@ -1339,8 +1339,8 @@
       <c r="F5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:11" ht="97.2">
       <c r="A6" s="32">
@@ -1361,8 +1361,8 @@
       <c r="F6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" spans="1:11" ht="97.2">
       <c r="A7" s="33">
@@ -1383,10 +1383,10 @@
       <c r="F7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="48"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:11" ht="81">
       <c r="A8" s="32">
@@ -1407,8 +1407,8 @@
       <c r="F8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="1:11" ht="97.2">
       <c r="A9" s="33">
@@ -1429,8 +1429,8 @@
       <c r="F9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:11" ht="97.2">
       <c r="A10" s="32">
@@ -1451,8 +1451,8 @@
       <c r="F10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:11" ht="49.2" thickBot="1">
       <c r="A11" s="34">
@@ -1473,8 +1473,8 @@
       <c r="F11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:11" ht="64.8">
       <c r="A12" s="32">
@@ -1495,8 +1495,8 @@
       <c r="F12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="1:11" ht="64.8">
       <c r="A13" s="33">
@@ -1517,8 +1517,8 @@
       <c r="F13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:11" ht="64.8">
       <c r="A14" s="32">
@@ -1539,8 +1539,8 @@
       <c r="F14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="1:11" ht="64.8">
       <c r="A15" s="33">
@@ -1561,8 +1561,8 @@
       <c r="F15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="44"/>
     </row>
     <row r="16" spans="1:11" ht="64.8">
       <c r="A16" s="32">
@@ -1583,8 +1583,8 @@
       <c r="F16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="1:28" ht="64.8">
       <c r="A17" s="33">
@@ -1605,8 +1605,8 @@
       <c r="F17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="1:28" ht="65.400000000000006" thickBot="1">
       <c r="A18" s="7">
@@ -1627,8 +1627,8 @@
       <c r="F18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="1:28" ht="64.8">
       <c r="A19" s="32">
@@ -1649,10 +1649,10 @@
       <c r="F19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="53"/>
+      <c r="H19" s="51"/>
     </row>
     <row r="20" spans="1:28" ht="64.8">
       <c r="A20" s="32">
@@ -1673,8 +1673,8 @@
       <c r="F20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21" spans="1:28" ht="49.2" thickBot="1">
       <c r="A21" s="37">
@@ -1695,8 +1695,8 @@
       <c r="F21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
     </row>
     <row r="22" spans="1:28" ht="65.400000000000006" thickBot="1">
       <c r="A22" s="38">
@@ -1717,8 +1717,8 @@
       <c r="F22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:28" ht="97.2">
       <c r="A23" s="32">
@@ -1739,8 +1739,8 @@
       <c r="F23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:28" ht="113.4">
       <c r="A24" s="32">
@@ -1761,8 +1761,8 @@
       <c r="F24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" spans="1:28" ht="81.599999999999994" thickBot="1">
       <c r="A25" s="34">
@@ -1783,8 +1783,8 @@
       <c r="F25" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
     </row>
     <row r="26" spans="1:28" ht="13.2">
       <c r="A26" s="35"/>
@@ -1797,16 +1797,16 @@
       <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:28" ht="28.5" customHeight="1">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="51"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
       <c r="K27" s="23"/>
@@ -1880,6 +1880,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G24:H24"/>
@@ -1896,16 +1906,6 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G7" location="BUG-00001!A1" display="BUG-00001"/>
@@ -1933,7 +1933,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="53.25" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="2" spans="1:7" ht="35.25" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="3" spans="1:7" ht="24.75" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="4" spans="1:7" ht="34.5" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="5" spans="1:7" ht="37.5" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="7" spans="1:7" ht="25.5" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="8" spans="1:7" ht="24.75" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="9" spans="1:7" ht="24.75" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>

</xml_diff>